<commit_message>
main (thiếu kho chứa)
abc
</commit_message>
<xml_diff>
--- a/Phân công công việc.xlsx
+++ b/Phân công công việc.xlsx
@@ -41,9 +41,6 @@
     <t>Xây dựng frmSach</t>
   </si>
   <si>
-    <t>Xây dựng frmQuanLyThe</t>
-  </si>
-  <si>
     <t>Xây dựng frmMuonTra</t>
   </si>
   <si>
@@ -90,6 +87,9 @@
   </si>
   <si>
     <t>Thêm , sửa , xóa</t>
+  </si>
+  <si>
+    <t>Xây dựng frmQuanLyKho</t>
   </si>
 </sst>
 </file>
@@ -492,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,7 +513,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
@@ -524,7 +524,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="6"/>
     </row>
@@ -536,7 +536,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="6"/>
     </row>
@@ -548,7 +548,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="6"/>
     </row>
@@ -557,10 +557,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="6"/>
     </row>
@@ -569,10 +569,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="6"/>
     </row>
@@ -581,13 +581,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
@@ -595,10 +595,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" s="6"/>
     </row>
@@ -607,10 +607,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="6"/>
     </row>
@@ -619,10 +619,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="6"/>
     </row>
@@ -631,10 +631,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" s="6"/>
     </row>
@@ -643,10 +643,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" s="6"/>
     </row>
@@ -655,10 +655,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="D13" s="6"/>
     </row>
@@ -667,10 +667,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D14" s="6"/>
     </row>

</xml_diff>

<commit_message>
Muon tra sach , phan quyen
xxx
</commit_message>
<xml_diff>
--- a/Phân công công việc.xlsx
+++ b/Phân công công việc.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkcuong\Documents\GitHub\TTNhom\QuanLyThuVien-HVKTQS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Phụ trách</t>
   </si>
@@ -36,9 +41,6 @@
     <t>Xây dựng frmSach</t>
   </si>
   <si>
-    <t>Xây dựng frmQuanLyThe</t>
-  </si>
-  <si>
     <t>Xây dựng frmMuonTra</t>
   </si>
   <si>
@@ -87,13 +89,13 @@
     <t>Thêm , sửa , xóa</t>
   </si>
   <si>
-    <t>chức năng Help</t>
+    <t>Xây dựng frmQuanLyKho</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -180,74 +182,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -264,10 +198,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="222222"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FAF9F9"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -548,7 +482,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -558,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +513,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
@@ -590,7 +524,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="6"/>
     </row>
@@ -602,7 +536,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="6"/>
     </row>
@@ -614,7 +548,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="6"/>
     </row>
@@ -623,10 +557,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="6"/>
     </row>
@@ -635,10 +569,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="6"/>
     </row>
@@ -647,13 +581,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
@@ -661,24 +595,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>22</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="6"/>
     </row>
@@ -687,10 +619,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="6"/>
     </row>
@@ -699,10 +631,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" s="6"/>
     </row>
@@ -711,10 +643,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" s="6"/>
     </row>
@@ -723,10 +655,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="D13" s="6"/>
     </row>
@@ -735,10 +667,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D14" s="6"/>
     </row>

</xml_diff>